<commit_message>
refactor 4: CMM045: them chuc nang in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF004_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF004_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF004_遅刻早退取消申請\二次\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94AD71F-938B-4E9D-85B1-7A8BA9485913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED489F7C-8903-4CA7-A119-5D771BCF247E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2523,7 +2523,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2696,7 +2696,7 @@
       <c r="K12" s="21"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="63.75" customHeight="1">
+    <row r="13" spans="1:12" ht="90" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="36"/>
       <c r="C13" s="37"/>

</xml_diff>

<commit_message>
refactor 4: KAF004: update hien thi checkbox
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF004_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF004_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF004_遅刻早退取消申請\二次\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED489F7C-8903-4CA7-A119-5D771BCF247E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="遅刻早退取消申請" sheetId="28" r:id="rId1"/>
@@ -65,19 +64,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -98,7 +97,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -464,11 +463,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="標準 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="標準 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="標準 3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="標準 10" xfId="2"/>
+    <cellStyle name="標準 2" xfId="1"/>
+    <cellStyle name="標準 2 2" xfId="4"/>
+    <cellStyle name="標準 3" xfId="3"/>
+    <cellStyle name="標準 3 2 2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -509,7 +508,7 @@
         <xdr:cNvPr id="37" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DBACEB5-F543-4483-842E-218F65C495BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7DBACEB5-F543-4483-842E-218F65C495BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -517,8 +516,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3162300" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="2819400" y="219075"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -528,7 +527,7 @@
           <xdr:cNvPr id="38" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774AC1B6-ADD8-4537-9467-B9D5C7CBB31E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{774AC1B6-ADD8-4537-9467-B9D5C7CBB31E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -582,7 +581,7 @@
           <xdr:cNvPr id="39" name="直線コネクタ 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DCE4C64-5D22-4E99-9999-DC016EC1DAAB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0DCE4C64-5D22-4E99-9999-DC016EC1DAAB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -622,7 +621,7 @@
           <xdr:cNvPr id="40" name="直線コネクタ 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D5EF830-9B46-4BE6-B3CC-5E087FD0393F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D5EF830-9B46-4BE6-B3CC-5E087FD0393F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -662,7 +661,7 @@
           <xdr:cNvPr id="41" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D925DC19-6E9D-4E61-94BF-8026FC57B81D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D925DC19-6E9D-4E61-94BF-8026FC57B81D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -700,13 +699,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t>  </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -715,7 +717,7 @@
           <xdr:cNvPr id="42" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55FB1446-3012-4C45-8207-003A54F5D9D6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55FB1446-3012-4C45-8207-003A54F5D9D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -753,13 +755,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -768,7 +773,7 @@
           <xdr:cNvPr id="43" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{292CBEB5-8103-4FEC-81B6-EDBAD97B8B66}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{292CBEB5-8103-4FEC-81B6-EDBAD97B8B66}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -806,13 +811,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -837,7 +845,7 @@
         <xdr:cNvPr id="44" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99C65A4F-B305-4076-838D-37B248F8FA15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{99C65A4F-B305-4076-838D-37B248F8FA15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -845,8 +853,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3778822" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3369247" y="219075"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -856,7 +864,7 @@
           <xdr:cNvPr id="45" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B62E5DB-A8A4-462B-AC9F-183B2757ECA9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B62E5DB-A8A4-462B-AC9F-183B2757ECA9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -910,7 +918,7 @@
           <xdr:cNvPr id="46" name="直線コネクタ 45">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7A7AF8E-A32B-4391-9E95-4073FDA6D27C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B7A7AF8E-A32B-4391-9E95-4073FDA6D27C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -950,7 +958,7 @@
           <xdr:cNvPr id="47" name="直線コネクタ 46">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E9B699-915B-4631-B1A8-1DB4C9883360}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{62E9B699-915B-4631-B1A8-1DB4C9883360}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -990,7 +998,7 @@
           <xdr:cNvPr id="48" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB721410-4459-41B8-A4BA-78F336ABFCFD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB721410-4459-41B8-A4BA-78F336ABFCFD}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1028,13 +1036,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1043,7 +1054,7 @@
           <xdr:cNvPr id="49" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00DF1DC0-FCAA-409E-B9C9-2DCECF7D2C5C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00DF1DC0-FCAA-409E-B9C9-2DCECF7D2C5C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1081,13 +1092,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1096,7 +1110,7 @@
           <xdr:cNvPr id="50" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEBD13E7-E109-4677-936B-83095C02C88F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DEBD13E7-E109-4677-936B-83095C02C88F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1134,13 +1148,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1165,7 +1182,7 @@
         <xdr:cNvPr id="51" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0450668D-643F-4C77-BE73-2EB18DB79E3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0450668D-643F-4C77-BE73-2EB18DB79E3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,8 +1190,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4403390" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3927140" y="219075"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1184,7 +1201,7 @@
           <xdr:cNvPr id="52" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20918DB7-DE6C-4E24-BEA2-143C48CE21DA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20918DB7-DE6C-4E24-BEA2-143C48CE21DA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1238,7 +1255,7 @@
           <xdr:cNvPr id="53" name="直線コネクタ 52">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78927FE4-DCCB-4F95-B479-8F37D0E4353A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78927FE4-DCCB-4F95-B479-8F37D0E4353A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1278,7 +1295,7 @@
           <xdr:cNvPr id="54" name="直線コネクタ 53">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90EBDE94-DF1F-4D9D-8D65-0BA56CA98205}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{90EBDE94-DF1F-4D9D-8D65-0BA56CA98205}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1318,7 +1335,7 @@
           <xdr:cNvPr id="55" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB2051D8-511D-45A8-B41E-3ABE12005E52}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB2051D8-511D-45A8-B41E-3ABE12005E52}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1356,13 +1373,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1371,7 +1391,7 @@
           <xdr:cNvPr id="56" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4010B74C-D45C-404A-963A-E9D94FBAC3BE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4010B74C-D45C-404A-963A-E9D94FBAC3BE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1409,13 +1429,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1424,7 +1447,7 @@
           <xdr:cNvPr id="57" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DDF2ECF-3EA1-4B4D-BE90-5347D121D0B4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1DDF2ECF-3EA1-4B4D-BE90-5347D121D0B4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1462,13 +1485,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1493,7 +1519,7 @@
         <xdr:cNvPr id="58" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D938DB9D-796C-44BD-8298-854AB4E99665}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D938DB9D-796C-44BD-8298-854AB4E99665}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,8 +1527,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5017073" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="4474148" y="219075"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1512,7 +1538,7 @@
           <xdr:cNvPr id="59" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0495346F-3259-4EE7-B4D6-EECD3E45B2D8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0495346F-3259-4EE7-B4D6-EECD3E45B2D8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1566,7 +1592,7 @@
           <xdr:cNvPr id="60" name="直線コネクタ 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56D24898-9F35-4857-B350-A976F1B928CC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56D24898-9F35-4857-B350-A976F1B928CC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1606,7 +1632,7 @@
           <xdr:cNvPr id="61" name="直線コネクタ 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBEC29BA-57A7-46B1-9E57-CB77619C1702}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EBEC29BA-57A7-46B1-9E57-CB77619C1702}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1646,7 +1672,7 @@
           <xdr:cNvPr id="62" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19DF3A87-A9DD-4C17-A315-9C83B113CB42}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{19DF3A87-A9DD-4C17-A315-9C83B113CB42}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1684,13 +1710,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1699,7 +1728,7 @@
           <xdr:cNvPr id="63" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6C72017-1283-4EF6-80D6-42CE5B59BAE9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6C72017-1283-4EF6-80D6-42CE5B59BAE9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1737,13 +1766,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1752,7 +1784,7 @@
           <xdr:cNvPr id="64" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDB45CB4-4AE2-453F-B1C4-DC3D53DE8F5A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BDB45CB4-4AE2-453F-B1C4-DC3D53DE8F5A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1790,13 +1822,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1821,7 +1856,7 @@
         <xdr:cNvPr id="100" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80BD5971-45E3-4D00-9C4E-298598D8740E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80BD5971-45E3-4D00-9C4E-298598D8740E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1829,8 +1864,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5641641" y="209550"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="5032041" y="209550"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1840,7 +1875,7 @@
           <xdr:cNvPr id="101" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC74AE4-B1AB-4237-8E40-255AABEC8DDE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCC74AE4-B1AB-4237-8E40-255AABEC8DDE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1894,7 +1929,7 @@
           <xdr:cNvPr id="102" name="直線コネクタ 101">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8013F66-A50D-44EB-86E4-804992290583}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D8013F66-A50D-44EB-86E4-804992290583}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1934,7 +1969,7 @@
           <xdr:cNvPr id="103" name="直線コネクタ 102">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4884B004-0B89-4ACB-A6EC-7F0607F111D1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4884B004-0B89-4ACB-A6EC-7F0607F111D1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1974,7 +2009,7 @@
           <xdr:cNvPr id="104" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB35953C-7198-4FC3-AEAD-4ED0148A0611}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB35953C-7198-4FC3-AEAD-4ED0148A0611}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2012,13 +2047,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2027,7 +2065,7 @@
           <xdr:cNvPr id="105" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC28F65-116F-4917-BCBB-386A3E23D9CF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CC28F65-116F-4917-BCBB-386A3E23D9CF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2065,13 +2103,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2080,7 +2121,7 @@
           <xdr:cNvPr id="106" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0BC4255-3B71-4F9F-A71D-99BA4043C01F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0BC4255-3B71-4F9F-A71D-99BA4043C01F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2118,13 +2159,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2519,23 +2563,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2184022B-8B52-4EAD-B846-0F9397241960}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.44140625" style="2"/>
+    <col min="18" max="16384" width="2.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">

</xml_diff>